<commit_message>
Excel sheet be pretty than old view and it was translated text of new functions
</commit_message>
<xml_diff>
--- a/root/static/results/users/results_1740566707.xlsx
+++ b/root/static/results/users/results_1740566707.xlsx
@@ -13,22 +13,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Sheet name: 2-variant | ID: 1740566707 | Jami yechganlar soni: 2</t>
-  </si>
-  <si>
-    <t>Nums</t>
-  </si>
-  <si>
-    <t>User Name</t>
-  </si>
-  <si>
-    <t>Correct Answers</t>
-  </si>
-  <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>Passed Time</t>
+    <t>Test nomi: 2-variant | Test id: 1740566707 | Jami yechganlar soni: 2</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>FOYDALANUVCHI</t>
+  </si>
+  <si>
+    <t>TO'G'RI JAVOBLAR</t>
+  </si>
+  <si>
+    <t>YIG'ILGAN BALL</t>
+  </si>
+  <si>
+    <t>TOPSHIRGAN VAQT</t>
   </si>
   <si>
     <t>Jack</t>
@@ -81,10 +81,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -429,69 +429,76 @@
   <dimension ref="A1:E5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="4" width="15" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>3.9</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>4</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>6.1</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>